<commit_message>
Added support form BMP180 temperature and pressure sensor
</commit_message>
<xml_diff>
--- a/register_map/output_struct.xlsx
+++ b/register_map/output_struct.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="135" uniqueCount="38">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="43">
   <si>
     <t xml:space="preserve">index</t>
   </si>
@@ -112,32 +112,7 @@
     <t xml:space="preserve">vbat</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">12-bit ADC reading of battery measurement N[11:0], </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">reference </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">R=0: 1.5 V, R=1: 2.5 V</t>
-    </r>
+    <t xml:space="preserve">12-bit ADC reading of battery measurement N[11:0], reference R=0: 1.5 V, R=1: 2.5 V</t>
   </si>
   <si>
     <t xml:space="preserve">N</t>
@@ -159,6 +134,21 @@
   </si>
   <si>
     <t xml:space="preserve">Si7021 temperature raw reading N</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bmp180_temperature</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BMP180 temperature reading in 0.1 degree Celsius</t>
+  </si>
+  <si>
+    <t xml:space="preserve">bmp180_pressure</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BMP180 pressure reading in Pascal</t>
   </si>
 </sst>
 </file>
@@ -168,7 +158,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="5">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -196,11 +186,6 @@
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="2"/>
     </font>
   </fonts>
   <fills count="2">
@@ -274,10 +259,10 @@
   <dimension ref="A1:U16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="118" zoomScaleNormal="118" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E12" activeCellId="0" sqref="E12"/>
+      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.62"/>
@@ -750,53 +735,77 @@
         <f aca="false">IF(AND(B8&gt;=2, MOD(B7+A7,2)=1),1,0)+A7+B7</f>
         <v>10</v>
       </c>
+      <c r="B8" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="C8" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="0" t="s">
+        <v>39</v>
+      </c>
+      <c r="E8" s="0" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="n">
         <f aca="false">IF(AND(B9&gt;=2, MOD(B8+A8,2)=1),1,0)+A8+B8</f>
-        <v>10</v>
+        <v>12</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C9" s="0" t="s">
+        <v>38</v>
+      </c>
+      <c r="D9" s="0" t="s">
+        <v>41</v>
+      </c>
+      <c r="E9" s="0" t="s">
+        <v>42</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="n">
         <f aca="false">IF(AND(B10&gt;=2, MOD(B9+A9,2)=1),1,0)+A9+B9</f>
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <f aca="false">IF(AND(B11&gt;=2, MOD(B10+A10,2)=1),1,0)+A10+B10</f>
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <f aca="false">IF(AND(B12&gt;=2, MOD(B11+A11,2)=1),1,0)+A11+B11</f>
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <f aca="false">IF(AND(B13&gt;=2, MOD(B12+A12,2)=1),1,0)+A12+B12</f>
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <f aca="false">IF(AND(B14&gt;=2, MOD(B13+A13,2)=1),1,0)+A13+B13</f>
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <f aca="false">IF(AND(B15&gt;=2, MOD(B14+A14,2)=1),1,0)+A14+B14</f>
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <f aca="false">IF(AND(B16&gt;=2, MOD(B15+A15,2)=1),1,0)+A15+B15</f>
-        <v>10</v>
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added support for a reed switch
</commit_message>
<xml_diff>
--- a/register_map/output_struct.xlsx
+++ b/register_map/output_struct.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="45">
   <si>
     <t xml:space="preserve">index</t>
   </si>
@@ -149,6 +149,12 @@
   </si>
   <si>
     <t xml:space="preserve">BMP180 pressure reading in Pascal</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reed</t>
+  </si>
+  <si>
+    <t xml:space="preserve">reed switch state: R[7:0]=0x00 (magnetic, L), R=0xAA (released, H)</t>
   </si>
 </sst>
 </file>
@@ -259,10 +265,10 @@
   <dimension ref="A1:U16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="118" zoomScaleNormal="118" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.62"/>
@@ -771,41 +777,101 @@
         <f aca="false">IF(AND(B10&gt;=2, MOD(B9+A9,2)=1),1,0)+A9+B9</f>
         <v>16</v>
       </c>
+      <c r="B10" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C10" s="0" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" s="0" t="s">
+        <v>43</v>
+      </c>
+      <c r="E10" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="H10" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="I10" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="K10" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="L10" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="M10" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="N10" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="O10" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="P10" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="Q10" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="R10" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="S10" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="T10" s="0" t="s">
+        <v>28</v>
+      </c>
+      <c r="U10" s="0" t="s">
+        <v>28</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="n">
         <f aca="false">IF(AND(B11&gt;=2, MOD(B10+A10,2)=1),1,0)+A10+B10</f>
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <f aca="false">IF(AND(B12&gt;=2, MOD(B11+A11,2)=1),1,0)+A11+B11</f>
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <f aca="false">IF(AND(B13&gt;=2, MOD(B12+A12,2)=1),1,0)+A12+B12</f>
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <f aca="false">IF(AND(B14&gt;=2, MOD(B13+A13,2)=1),1,0)+A13+B13</f>
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <f aca="false">IF(AND(B15&gt;=2, MOD(B14+A14,2)=1),1,0)+A14+B14</f>
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <f aca="false">IF(AND(B16&gt;=2, MOD(B15+A15,2)=1),1,0)+A15+B15</f>
-        <v>16</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added server, write incoming data to database
</commit_message>
<xml_diff>
--- a/register_map/output_struct.xlsx
+++ b/register_map/output_struct.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="160" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="48">
   <si>
     <t xml:space="preserve">index</t>
   </si>
@@ -31,6 +31,9 @@
     <t xml:space="preserve">type</t>
   </si>
   <si>
+    <t xml:space="preserve">sql_type</t>
+  </si>
+  <si>
     <t xml:space="preserve">field</t>
   </si>
   <si>
@@ -88,6 +91,9 @@
     <t xml:space="preserve">u</t>
   </si>
   <si>
+    <t xml:space="preserve">INTEGER</t>
+  </si>
+  <si>
     <t xml:space="preserve">addr</t>
   </si>
   <si>
@@ -107,6 +113,9 @@
   </si>
   <si>
     <t xml:space="preserve">R</t>
+  </si>
+  <si>
+    <t xml:space="preserve">REAL</t>
   </si>
   <si>
     <t xml:space="preserve">vbat</t>
@@ -262,18 +271,19 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:U16"/>
+  <dimension ref="A1:V16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="118" zoomScaleNormal="118" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E11" activeCellId="0" sqref="E11"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="118" zoomScaleNormal="118" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.62"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="71.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="21" min="6" style="0" width="4.1"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="18.88"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="71.33"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="22" min="7" style="0" width="4.1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -340,6 +350,9 @@
       <c r="U1" s="1" t="s">
         <v>20</v>
       </c>
+      <c r="V1" s="1" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="n">
@@ -349,61 +362,64 @@
         <v>1</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J2" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K2" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="L2" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="M2" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="N2" s="0" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="O2" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="P2" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="Q2" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="R2" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="S2" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="T2" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="U2" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
+      </c>
+      <c r="V2" s="0" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -415,64 +431,67 @@
         <v>1</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>26</v>
+        <v>23</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>24</v>
+        <v>29</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J3" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="K3" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="L3" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="M3" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="N3" s="0" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="O3" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="P3" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Q3" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="R3" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="S3" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="T3" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="U3" s="0" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="4" customFormat="false" ht="13.1" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+        <v>30</v>
+      </c>
+      <c r="V3" s="0" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="n">
         <f aca="false">IF(AND(B4&gt;=2, MOD(B3+A3,2)=1),1,0)+A3+B3</f>
         <v>2</v>
@@ -481,61 +500,64 @@
         <v>2</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J4" s="0" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="K4" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="L4" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="M4" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="N4" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="O4" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="P4" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="Q4" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="R4" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="S4" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="T4" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="U4" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
+      </c>
+      <c r="V4" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -547,61 +569,64 @@
         <v>2</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>24</v>
+        <v>36</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="J5" s="0" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="K5" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="L5" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="M5" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="N5" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="O5" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="P5" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="Q5" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="R5" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="S5" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="T5" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="U5" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
+      </c>
+      <c r="V5" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -613,61 +638,64 @@
         <v>2</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>31</v>
+        <v>38</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="J6" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="K6" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="L6" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="M6" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="N6" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="O6" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="P6" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="Q6" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="R6" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="S6" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="T6" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="U6" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
+      </c>
+      <c r="V6" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -679,61 +707,64 @@
         <v>2</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>31</v>
+        <v>40</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="J7" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="K7" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="L7" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="M7" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="N7" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="O7" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="P7" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="Q7" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="R7" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="S7" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="T7" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="U7" s="0" t="s">
-        <v>31</v>
+        <v>34</v>
+      </c>
+      <c r="V7" s="0" t="s">
+        <v>34</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -745,13 +776,16 @@
         <v>2</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
+      </c>
+      <c r="F8" s="0" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -763,13 +797,16 @@
         <v>4</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>38</v>
+        <v>41</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>41</v>
+        <v>31</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="F9" s="0" t="s">
+        <v>45</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -781,61 +818,64 @@
         <v>1</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>43</v>
+        <v>23</v>
       </c>
       <c r="E10" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="F10" s="0" t="s">
-        <v>28</v>
+        <v>47</v>
       </c>
       <c r="G10" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="H10" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="I10" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="J10" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="K10" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="L10" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="M10" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="N10" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="O10" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="P10" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="Q10" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="R10" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="S10" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="T10" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="U10" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
+      </c>
+      <c r="V10" s="0" t="s">
+        <v>30</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Added receiver RSSI value to out_regs and database
</commit_message>
<xml_diff>
--- a/register_map/output_struct.xlsx
+++ b/register_map/output_struct.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="50">
   <si>
     <t xml:space="preserve">index</t>
   </si>
@@ -164,6 +164,12 @@
   </si>
   <si>
     <t xml:space="preserve">reed switch state: R[7:0]=0x00 (magnetic, L), R=0xAA (released, H)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">rssi</t>
+  </si>
+  <si>
+    <t xml:space="preserve">RSSI reading for receiver</t>
   </si>
 </sst>
 </file>
@@ -274,10 +280,10 @@
   <dimension ref="A1:V16"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B1" colorId="64" zoomScale="118" zoomScaleNormal="118" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D11" activeCellId="0" sqref="D11"/>
+      <selection pane="topLeft" activeCell="D12" activeCellId="0" sqref="D12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="5.39"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="5.62"/>
@@ -883,35 +889,50 @@
         <f aca="false">IF(AND(B11&gt;=2, MOD(B10+A10,2)=1),1,0)+A10+B10</f>
         <v>17</v>
       </c>
+      <c r="B11" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="C11" s="0" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11" s="0" t="s">
+        <v>31</v>
+      </c>
+      <c r="E11" s="0" t="s">
+        <v>48</v>
+      </c>
+      <c r="F11" s="0" t="s">
+        <v>49</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="n">
         <f aca="false">IF(AND(B12&gt;=2, MOD(B11+A11,2)=1),1,0)+A11+B11</f>
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="n">
         <f aca="false">IF(AND(B13&gt;=2, MOD(B12+A12,2)=1),1,0)+A12+B12</f>
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="n">
         <f aca="false">IF(AND(B14&gt;=2, MOD(B13+A13,2)=1),1,0)+A13+B13</f>
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="n">
         <f aca="false">IF(AND(B15&gt;=2, MOD(B14+A14,2)=1),1,0)+A14+B14</f>
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="n">
         <f aca="false">IF(AND(B16&gt;=2, MOD(B15+A15,2)=1),1,0)+A15+B15</f>
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>